<commit_message>
Fix spurious space for Alfredo
</commit_message>
<xml_diff>
--- a/11-CollaborationList/CNRS-Orsay.xlsx
+++ b/11-CollaborationList/CNRS-Orsay.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://api.box.com/wopi/files/2050112243709/WOPIServiceId_TP_BOX_2/WOPIUserId_-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:9_{A4525352-3B6E-E34D-84BC-C622496379D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57FA2057-753F-2D44-86ED-F445C3CFDE7C}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:9_{A4525352-3B6E-E34D-84BC-C622496379D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D0022A6-7E8D-7442-B180-632E23FF2273}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{AD094988-A457-9044-86A1-58DE43D24A21}"/>
   </bookViews>
@@ -88,9 +88,6 @@
     <t>Alfredo Fernandez-Rodriguez</t>
   </si>
   <si>
-    <t>A. </t>
-  </si>
-  <si>
     <t>alfredo.fernandez-rodriguez@universite-paris-saclay.fr; alfredofernandezrod@gmail.com</t>
   </si>
   <si>
@@ -98,6 +95,9 @@
   </si>
   <si>
     <t>Institut des Sciences Moléculaires d'Orsay, Rue André Rivière, Bâtiment 520, 91400 Orsay, France</t>
+  </si>
+  <si>
+    <t>A.</t>
   </si>
 </sst>
 </file>
@@ -593,10 +593,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1000,7 +1001,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1083,20 +1084,20 @@
       <c r="C2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="I2" s="1">
         <v>1</v>

</xml_diff>